<commit_message>
Update Dependencies & Add Image
</commit_message>
<xml_diff>
--- a/resource/Data.xlsx
+++ b/resource/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Undisclosed\Capstone Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\[P]roject\Github\Project\Streamlit-Tetris\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374EFFF3-4ED9-44A4-86CF-6346ACD1A975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634CCFAD-0D64-4A8F-BDC9-5B143B1878AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{B6E8FAAF-E45E-4946-8B39-8972A4FD321A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11040" activeTab="2" xr2:uid="{B6E8FAAF-E45E-4946-8B39-8972A4FD321A}"/>
   </bookViews>
   <sheets>
     <sheet name="Norway" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -42,27 +44,6 @@
     <t>Transportasi Darat</t>
   </si>
   <si>
-    <t>Pembakaran Industri</t>
-  </si>
-  <si>
-    <t>Pembakaran Domestik</t>
-  </si>
-  <si>
-    <t>Pembangkit Listrik &amp; Pemanas</t>
-  </si>
-  <si>
-    <t>Transportasi</t>
-  </si>
-  <si>
-    <t>Industri</t>
-  </si>
-  <si>
-    <t>Domestik</t>
-  </si>
-  <si>
-    <t>PL &amp; Pemanas</t>
-  </si>
-  <si>
     <t>Penyebab</t>
   </si>
   <si>
@@ -93,9 +74,6 @@
     <t>Toyota Rush GR Sport MT</t>
   </si>
   <si>
-    <t>Bensin</t>
-  </si>
-  <si>
     <t>TOYOTA All New Avanza 1.5 G 2021</t>
   </si>
   <si>
@@ -126,9 +104,6 @@
     <t>Hyundai Ioniq5 Signature Extended</t>
   </si>
   <si>
-    <t>Elektrik</t>
-  </si>
-  <si>
     <t>NISSAN Leaf</t>
   </si>
   <si>
@@ -163,6 +138,33 @@
   </si>
   <si>
     <t>Norways EV Vehicle Market Share (%)</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Domestic</t>
+  </si>
+  <si>
+    <t>PP &amp; Heater</t>
+  </si>
+  <si>
+    <t>Power Plant &amp; Heater</t>
+  </si>
+  <si>
+    <t>Domestic Burning</t>
+  </si>
+  <si>
+    <t>Industrial Smoke</t>
+  </si>
+  <si>
+    <t>Elektric</t>
+  </si>
+  <si>
+    <t>Gasoline</t>
   </si>
 </sst>
 </file>
@@ -563,27 +565,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{329E1D78-0447-45D1-AD26-EF21DC7CE8EB}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D15:D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>2009</v>
       </c>
@@ -594,7 +596,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2010</v>
       </c>
@@ -605,7 +607,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2011</v>
       </c>
@@ -616,7 +618,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>2012</v>
       </c>
@@ -627,7 +629,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2013</v>
       </c>
@@ -638,7 +640,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2014</v>
       </c>
@@ -649,7 +651,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>2015</v>
       </c>
@@ -660,7 +662,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>2016</v>
       </c>
@@ -671,7 +673,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>2017</v>
       </c>
@@ -682,7 +684,7 @@
         <v>33.6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>2018</v>
       </c>
@@ -693,7 +695,7 @@
         <v>49.1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>2019</v>
       </c>
@@ -704,7 +706,7 @@
         <v>55.9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>2020</v>
       </c>
@@ -726,27 +728,27 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="15.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.54296875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="15.36328125" style="1"/>
+    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="15.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -754,40 +756,40 @@
         <v>75</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B3" s="4">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4">
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B5" s="4">
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -799,46 +801,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE399D4-2C37-4B62-ABFB-A89AF2DE162C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.1796875" customWidth="1"/>
+    <col min="1" max="1" width="51.140625" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="16.08984375" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="C2" s="6">
         <v>291500000</v>
@@ -847,18 +849,18 @@
         <v>14.28</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F2" s="6">
         <v>535.71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C3" s="6">
         <v>232850000</v>
@@ -867,18 +869,18 @@
         <v>11.5</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F3" s="6">
         <v>665.22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C4" s="6">
         <v>278100000</v>
@@ -887,18 +889,18 @@
         <v>12</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F4" s="6">
         <v>637.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C5" s="6">
         <v>302200000</v>
@@ -907,18 +909,18 @@
         <v>14.28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F5" s="6">
         <v>535.71</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C6" s="6">
         <v>309100000</v>
@@ -927,18 +929,18 @@
         <v>12.6</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F6" s="6">
         <v>607.14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6">
         <v>677000000</v>
@@ -947,18 +949,18 @@
         <v>6.21</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F7" s="6">
         <v>397.1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6">
         <v>649000000</v>
@@ -967,18 +969,18 @@
         <v>6.79</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F8" s="6">
         <v>363.18</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C9" s="6">
         <v>677000000</v>
@@ -987,18 +989,18 @@
         <v>8.1460000000000008</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F9" s="6">
         <v>302.73</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C10" s="6">
         <v>697000000</v>
@@ -1007,18 +1009,18 @@
         <v>7.78</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F10" s="6">
         <v>316.97000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C11" s="6">
         <f>AVERAGE(C7:C10)</f>
@@ -1029,19 +1031,19 @@
         <v>7.2315000000000005</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
         <v>344.995</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C12" s="6">
         <f>AVERAGE(C2:C6)</f>
@@ -1052,7 +1054,7 @@
         <v>12.931999999999999</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="1"/>

</xml_diff>